<commit_message>
feat: validator cnpj in inputs
</commit_message>
<xml_diff>
--- a/inputs.xlsx
+++ b/inputs.xlsx
@@ -68,12 +68,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -381,13 +384,13 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:A161"/>
+  <dimension ref="A1:A162"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="3" width="19.14785714285714" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="4" width="19.14785714285714" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
@@ -410,34 +413,36 @@
         <v>30609801000110</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
-      <c r="A5" s="1">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="16.5">
+      <c r="A5" s="3">
+        <v>123</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
+      <c r="A6" s="1">
         <v>27169224000188</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
-      <c r="A6" s="1">
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
+      <c r="A7" s="1">
         <v>24259650000114</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
-      <c r="A7" s="1">
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
+      <c r="A8" s="1">
         <v>26719700000124</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
-      <c r="A8" s="1">
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
+      <c r="A9" s="1">
         <v>30745496000193</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
-      <c r="A9" s="1">
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
+      <c r="A10" s="1">
         <v>17186864000142</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
-      <c r="A10" s="1"/>
-    </row>
     <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
       <c r="A11" s="1"/>
     </row>
@@ -498,7 +503,7 @@
     <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="18.75">
       <c r="A30" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="16.5">
+    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="18.75">
       <c r="A31" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="16.5">
@@ -890,6 +895,9 @@
     </row>
     <row x14ac:dyDescent="0.25" r="161" customHeight="1" ht="16.5">
       <c r="A161" s="1"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="162" customHeight="1" ht="16.5">
+      <c r="A162" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>